<commit_message>
Corrección de errores: Pruebas alterando la lista de productos
</commit_message>
<xml_diff>
--- a/Requerimiento_Productos.xlsx
+++ b/Requerimiento_Productos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Programación\Python\Pruebas_WebScraping\Búsqueda Mercado Público\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3230FC-EB7A-4FD2-9B81-5F28A3A4B37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0400E6A8-2EAE-407C-97DA-38D19F6D039F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64CE2681-56B1-4764-AF32-1FB6686227D7}"/>
   </bookViews>
@@ -603,7 +603,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,12 +900,12 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G7" r:id="rId1" xr:uid="{11DE7B76-C796-4417-8D68-3BC5E85A1939}"/>
-    <hyperlink ref="G5" r:id="rId2" xr:uid="{B5DF10FF-9F1A-4BCF-8A14-3912A227CC1A}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{B7EF0633-2DE2-4D35-AD67-834D7AE5987C}"/>
-    <hyperlink ref="G2" r:id="rId4" xr:uid="{1C6D48D2-3579-4DFE-BD2D-5E2047D9DE0D}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{52383767-9EE1-42DE-864F-CAB8082D0D93}"/>
-    <hyperlink ref="G6" r:id="rId6" xr:uid="{109A2D06-341A-4CAB-B4D7-E3E41648260C}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{9FEC74CC-7EAE-4F53-AB64-9CA3F1EAAA74}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{B7EF0633-2DE2-4D35-AD67-834D7AE5987C}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{109A2D06-341A-4CAB-B4D7-E3E41648260C}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{9FEC74CC-7EAE-4F53-AB64-9CA3F1EAAA74}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{B5DF10FF-9F1A-4BCF-8A14-3912A227CC1A}"/>
+    <hyperlink ref="G2" r:id="rId6" xr:uid="{1C6D48D2-3579-4DFE-BD2D-5E2047D9DE0D}"/>
+    <hyperlink ref="G3" r:id="rId7" xr:uid="{52383767-9EE1-42DE-864F-CAB8082D0D93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>